<commit_message>
customer login page added
</commit_message>
<xml_diff>
--- a/Main Assignment Maven/Xyzbank/src/main/java/com/xyzbank/qa/testdata/CustomerData.xlsx
+++ b/Main Assignment Maven/Xyzbank/src/main/java/com/xyzbank/qa/testdata/CustomerData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udayprsingh\IdeaProjects\Xyzbank\src\main\java\com\xyzbank\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CC1AAA-9889-40B9-A480-7498ED32C534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640F06C8-D73F-4644-82A0-03A658ABEFF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFA861AF-EA3C-4DB8-9AE1-D4D33A748D5A}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>